<commit_message>
hybrid model test on new value-driven dataset
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-14.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-14.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="neg vs pos" sheetId="1" r:id="rId1"/>
+    <sheet name="hybrid model" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -64,6 +65,18 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-43 (positive flow).csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-43.csv)</t>
+  </si>
+  <si>
+    <t>f1</t>
+  </si>
+  <si>
+    <t>Hybrid model 3 (superdataset-43.csv)</t>
+  </si>
+  <si>
+    <t>Значимость</t>
   </si>
 </sst>
 </file>
@@ -540,7 +553,314 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'hybrid model'!$W$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Значимость</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'hybrid model'!$V$4:$V$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>library</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cultureorg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>musartschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'hybrid model'!$W$4:$W$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.4658653219200407E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.6762021118089672E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5697851520440052E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46472624855624489</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33472872605610132</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.342649952992358E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D94C-4D78-A2A4-02A5DC8635B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="716856271"/>
+        <c:axId val="716856687"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="716856271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="716856687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="716856687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="716856271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1099,6 +1419,525 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1110,13 +1949,48 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1399,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:S57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2654,4 +3528,1620 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:W57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q36" sqref="Q36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="21" max="21" width="10.28515625" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="V3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="V4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="3">
+        <v>4.4658653219200407E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
+        <v>46.48147046563912</v>
+      </c>
+      <c r="F5" s="3">
+        <v>120.72817482419769</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>40.425659637723882</v>
+      </c>
+      <c r="K5" s="3">
+        <v>115.5372575464111</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.9767441860465117</v>
+      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="V5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="W5" s="3">
+        <v>8.6762021118089672E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <f>D5+1</f>
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>46.348891771824249</v>
+      </c>
+      <c r="F6" s="3">
+        <v>118.8060567685044</v>
+      </c>
+      <c r="I6" s="2">
+        <f>I5+1</f>
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
+        <v>40.804415747470678</v>
+      </c>
+      <c r="K6" s="3">
+        <v>111.2756729275292</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.9629629629629628</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="V6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="3">
+        <v>5.5697851520440052E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D7" s="2">
+        <f t="shared" ref="D7:D54" si="0">D6+1</f>
+        <v>3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>46.29241870705475</v>
+      </c>
+      <c r="F7" s="3">
+        <v>120.42846598165529</v>
+      </c>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I54" si="1">I6+1</f>
+        <v>3</v>
+      </c>
+      <c r="J7" s="3">
+        <v>41.126737584709247</v>
+      </c>
+      <c r="K7" s="3">
+        <v>109.4415373828204</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.98349834983498341</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="V7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0.46472624855624489</v>
+      </c>
+    </row>
+    <row r="8" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45.939887527501227</v>
+      </c>
+      <c r="F8" s="3">
+        <v>120.240568711527</v>
+      </c>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="J8" s="3">
+        <v>41.207408996447761</v>
+      </c>
+      <c r="K8" s="3">
+        <v>108.529471682037</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.98017621145374445</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="V8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0.33472872605610132</v>
+      </c>
+    </row>
+    <row r="9" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>46.250764983510287</v>
+      </c>
+      <c r="F9" s="3">
+        <v>118.79719214424151</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>41.365896942628112</v>
+      </c>
+      <c r="K9" s="3">
+        <v>110.1957415405943</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0.97104677060133626</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="V9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="W9" s="3">
+        <v>1.342649952992358E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>45.922376146443888</v>
+      </c>
+      <c r="F10" s="3">
+        <v>119.4353011497568</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J10" s="3">
+        <v>41.157659790836483</v>
+      </c>
+      <c r="K10" s="3">
+        <v>111.6295385689218</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.97136563876651971</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E11" s="3">
+        <v>46.320949619095359</v>
+      </c>
+      <c r="F11" s="3">
+        <v>116.9587571794836</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J11" s="3">
+        <v>40.475915502344847</v>
+      </c>
+      <c r="K11" s="3">
+        <v>113.6215393556363</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.97339246119733924</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E12" s="3">
+        <v>46.136558619464097</v>
+      </c>
+      <c r="F12" s="3">
+        <v>123.0774856010012</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J12" s="3">
+        <v>41.010063919573582</v>
+      </c>
+      <c r="K12" s="3">
+        <v>109.0555069922451</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.9735682819383259</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E13" s="3">
+        <v>46.152640870645122</v>
+      </c>
+      <c r="F13" s="3">
+        <v>119.5447872764246</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="J13" s="3">
+        <v>41.228014257862633</v>
+      </c>
+      <c r="K13" s="3">
+        <v>110.1325283550843</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.95964125560538116</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+    </row>
+    <row r="14" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E14" s="3">
+        <v>46.105429014827308</v>
+      </c>
+      <c r="F14" s="3">
+        <v>115.8938171657983</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J14" s="3">
+        <v>41.582277380464546</v>
+      </c>
+      <c r="K14" s="3">
+        <v>109.845801856607</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.95739910313901333</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E15" s="3">
+        <v>46.257596755809352</v>
+      </c>
+      <c r="F15" s="3">
+        <v>117.1430853812311</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="J15" s="3">
+        <v>41.006369859646753</v>
+      </c>
+      <c r="K15" s="3">
+        <v>111.8492429290979</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0.97333333333333327</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45.687557419359692</v>
+      </c>
+      <c r="F16" s="3">
+        <v>121.2638497157094</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="J16" s="3">
+        <v>40.846949188810449</v>
+      </c>
+      <c r="K16" s="3">
+        <v>114.0120904825412</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.96444444444444444</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="E17" s="3">
+        <v>45.712831093695208</v>
+      </c>
+      <c r="F17" s="3">
+        <v>119.6662859669559</v>
+      </c>
+      <c r="I17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="J17" s="3">
+        <v>41.224960533545293</v>
+      </c>
+      <c r="K17" s="3">
+        <v>108.8696515474297</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.9780219780219781</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="E18" s="3">
+        <v>46.49417304919892</v>
+      </c>
+      <c r="F18" s="3">
+        <v>116.375020743581</v>
+      </c>
+      <c r="I18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="J18" s="3">
+        <v>41.329713783888863</v>
+      </c>
+      <c r="K18" s="3">
+        <v>110.0578750970451</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.97362637362637361</v>
+      </c>
+      <c r="O18" s="2"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E19" s="3">
+        <v>45.915327624042703</v>
+      </c>
+      <c r="F19" s="3">
+        <v>118.12273943852099</v>
+      </c>
+      <c r="I19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="J19" s="3">
+        <v>41.165720984487493</v>
+      </c>
+      <c r="K19" s="3">
+        <v>107.53254502907819</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.97782705099778278</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E20" s="3">
+        <v>45.708870307874029</v>
+      </c>
+      <c r="F20" s="3">
+        <v>124.2963666611075</v>
+      </c>
+      <c r="I20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J20" s="3">
+        <v>41.124175369940978</v>
+      </c>
+      <c r="K20" s="3">
+        <v>107.561437897289</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.97464167585446526</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="E21" s="3">
+        <v>45.855539884259287</v>
+      </c>
+      <c r="F21" s="3">
+        <v>121.076573269612</v>
+      </c>
+      <c r="I21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="J21" s="3">
+        <v>41.271222767021968</v>
+      </c>
+      <c r="K21" s="3">
+        <v>109.4760116425679</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0.96674057649667411</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="E22" s="3">
+        <v>46.069464359715433</v>
+      </c>
+      <c r="F22" s="3">
+        <v>121.1006253991313</v>
+      </c>
+      <c r="I22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="J22" s="3">
+        <v>41.006196869306848</v>
+      </c>
+      <c r="K22" s="3">
+        <v>110.4420654321809</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0.97787610619469023</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+    </row>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E23" s="3">
+        <v>45.810171752264402</v>
+      </c>
+      <c r="F23" s="3">
+        <v>119.7282576217341</v>
+      </c>
+      <c r="I23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="J23" s="3">
+        <v>40.757167197986533</v>
+      </c>
+      <c r="K23" s="3">
+        <v>113.2267329073251</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.97231450719822821</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+    </row>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E24" s="3">
+        <v>46.079507693756597</v>
+      </c>
+      <c r="F24" s="3">
+        <v>119.7895356835173</v>
+      </c>
+      <c r="I24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="J24" s="3">
+        <v>40.616479058394127</v>
+      </c>
+      <c r="K24" s="3">
+        <v>115.3936085452532</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.96909492273730691</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+    </row>
+    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E25" s="3">
+        <v>45.757533575072891</v>
+      </c>
+      <c r="F25" s="3">
+        <v>120.9448188627161</v>
+      </c>
+      <c r="I25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="J25" s="3">
+        <v>40.346030222739223</v>
+      </c>
+      <c r="K25" s="3">
+        <v>113.15104345400169</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.97458563535911602</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+    </row>
+    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="E26" s="3">
+        <v>45.988429949916863</v>
+      </c>
+      <c r="F26" s="3">
+        <v>121.4634271299158</v>
+      </c>
+      <c r="I26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="J26" s="3">
+        <v>40.54440950199799</v>
+      </c>
+      <c r="K26" s="3">
+        <v>112.5438502564962</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.96559378468368484</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+    </row>
+    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E27" s="3">
+        <v>46.252933885792487</v>
+      </c>
+      <c r="F27" s="3">
+        <v>116.1884406241326</v>
+      </c>
+      <c r="I27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J27" s="3">
+        <v>41.041257434129612</v>
+      </c>
+      <c r="K27" s="3">
+        <v>111.00106082579001</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0.96188340807174888</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+    </row>
+    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E28" s="3">
+        <v>46.060513682073868</v>
+      </c>
+      <c r="F28" s="3">
+        <v>122.2294380011146</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="J28" s="3">
+        <v>40.48956828115962</v>
+      </c>
+      <c r="K28" s="3">
+        <v>115.77199233389941</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0.97111111111111115</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+    </row>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="E29" s="3">
+        <v>46.290904574294203</v>
+      </c>
+      <c r="F29" s="3">
+        <v>119.2183559048124</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J29" s="3">
+        <v>41.127671556623547</v>
+      </c>
+      <c r="K29" s="3">
+        <v>112.0676572536286</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0.97362637362637361</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+    </row>
+    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="E30" s="3">
+        <v>45.586773385357738</v>
+      </c>
+      <c r="F30" s="3">
+        <v>121.4658369542242</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="J30" s="3">
+        <v>40.76063880030901</v>
+      </c>
+      <c r="K30" s="3">
+        <v>113.2048272898456</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0.96666666666666667</v>
+      </c>
+      <c r="O30" s="2"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+    </row>
+    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="E31" s="3">
+        <v>46.587967409588771</v>
+      </c>
+      <c r="F31" s="3">
+        <v>115.9465852901378</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="J31" s="3">
+        <v>40.517697125278929</v>
+      </c>
+      <c r="K31" s="3">
+        <v>112.7177995746451</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0.96345514950166111</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+    </row>
+    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E32" s="3">
+        <v>45.626259615917981</v>
+      </c>
+      <c r="F32" s="3">
+        <v>121.9799426153988</v>
+      </c>
+      <c r="I32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="J32" s="3">
+        <v>40.381142815401113</v>
+      </c>
+      <c r="K32" s="3">
+        <v>112.6234970965933</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0.97243660418963607</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45.795561511404998</v>
+      </c>
+      <c r="F33" s="3">
+        <v>124.8188533286234</v>
+      </c>
+      <c r="I33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="J33" s="3">
+        <v>40.683040636818824</v>
+      </c>
+      <c r="K33" s="3">
+        <v>116.0150087430478</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0.97104677060133626</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E34" s="3">
+        <v>45.912739030614183</v>
+      </c>
+      <c r="F34" s="3">
+        <v>120.5808759561165</v>
+      </c>
+      <c r="I34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J34" s="3">
+        <v>40.857174006962921</v>
+      </c>
+      <c r="K34" s="3">
+        <v>114.14596984009989</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0.96559378468368484</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="E35" s="3">
+        <v>46.33324863766304</v>
+      </c>
+      <c r="F35" s="3">
+        <v>120.4973480058193</v>
+      </c>
+      <c r="I35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="J35" s="3">
+        <v>40.701149745289861</v>
+      </c>
+      <c r="K35" s="3">
+        <v>112.99270738974231</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0.97905181918412354</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+    </row>
+    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="E36" s="3">
+        <v>45.865435238285059</v>
+      </c>
+      <c r="F36" s="3">
+        <v>123.3981328288157</v>
+      </c>
+      <c r="I36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="J36" s="3">
+        <v>40.530863783699793</v>
+      </c>
+      <c r="K36" s="3">
+        <v>112.04175359435651</v>
+      </c>
+      <c r="L36" s="3">
+        <v>0.967741935483871</v>
+      </c>
+      <c r="O36" s="2"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="E37" s="3">
+        <v>46.109763003882883</v>
+      </c>
+      <c r="F37" s="3">
+        <v>121.1376732703399</v>
+      </c>
+      <c r="I37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="J37" s="3">
+        <v>40.928839892560923</v>
+      </c>
+      <c r="K37" s="3">
+        <v>111.84494957648521</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0.97560975609756095</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="E38" s="3">
+        <v>46.042229290613342</v>
+      </c>
+      <c r="F38" s="3">
+        <v>119.11981346420021</v>
+      </c>
+      <c r="I38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="J38" s="3">
+        <v>40.829773289505773</v>
+      </c>
+      <c r="K38" s="3">
+        <v>113.1596073214688</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0.9656699889258028</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E39" s="3">
+        <v>45.732652490600991</v>
+      </c>
+      <c r="F39" s="3">
+        <v>124.01655881236429</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="J39" s="3">
+        <v>40.856763566558463</v>
+      </c>
+      <c r="K39" s="3">
+        <v>112.93681768072059</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0.96412556053811649</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="E40" s="3">
+        <v>46.002989974556392</v>
+      </c>
+      <c r="F40" s="3">
+        <v>120.10664119674949</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="J40" s="3">
+        <v>40.711702121408841</v>
+      </c>
+      <c r="K40" s="3">
+        <v>110.2697438985325</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0.97016574585635351</v>
+      </c>
+      <c r="O40" s="2"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E41" s="3">
+        <v>45.639223259654429</v>
+      </c>
+      <c r="F41" s="3">
+        <v>122.7213527185388</v>
+      </c>
+      <c r="I41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="J41" s="3">
+        <v>41.105913896950277</v>
+      </c>
+      <c r="K41" s="3">
+        <v>109.4765103496659</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0.9767441860465117</v>
+      </c>
+      <c r="O41" s="2"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+    </row>
+    <row r="42" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E42" s="3">
+        <v>45.872299836613983</v>
+      </c>
+      <c r="F42" s="3">
+        <v>119.93662101771849</v>
+      </c>
+      <c r="I42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="J42" s="3">
+        <v>40.701272642608387</v>
+      </c>
+      <c r="K42" s="3">
+        <v>114.1951644301591</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0.96551724137931028</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+    </row>
+    <row r="43" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="E43" s="3">
+        <v>45.744197531120783</v>
+      </c>
+      <c r="F43" s="3">
+        <v>124.7914650234022</v>
+      </c>
+      <c r="I43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="J43" s="3">
+        <v>40.890373024700096</v>
+      </c>
+      <c r="K43" s="3">
+        <v>110.74205893973991</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0.9767441860465117</v>
+      </c>
+      <c r="O43" s="2"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+    </row>
+    <row r="44" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E44" s="3">
+        <v>46.128079299635367</v>
+      </c>
+      <c r="F44" s="3">
+        <v>121.2293029343903</v>
+      </c>
+      <c r="I44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J44" s="3">
+        <v>40.725513849705742</v>
+      </c>
+      <c r="K44" s="3">
+        <v>113.11172933147979</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0.96071829405162745</v>
+      </c>
+      <c r="O44" s="2"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+    </row>
+    <row r="45" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E45" s="3">
+        <v>46.360743832447817</v>
+      </c>
+      <c r="F45" s="3">
+        <v>118.3992535160796</v>
+      </c>
+      <c r="I45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="J45" s="3">
+        <v>40.825046529467187</v>
+      </c>
+      <c r="K45" s="3">
+        <v>111.733357684745</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0.967741935483871</v>
+      </c>
+      <c r="O45" s="2"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+    </row>
+    <row r="46" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E46" s="3">
+        <v>46.154807779893581</v>
+      </c>
+      <c r="F46" s="3">
+        <v>118.500510212636</v>
+      </c>
+      <c r="I46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="J46" s="3">
+        <v>41.323526379498183</v>
+      </c>
+      <c r="K46" s="3">
+        <v>106.16300548881389</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0.96636771300448432</v>
+      </c>
+      <c r="O46" s="2"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+    </row>
+    <row r="47" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="E47" s="3">
+        <v>46.309614951410431</v>
+      </c>
+      <c r="F47" s="3">
+        <v>119.83761652589421</v>
+      </c>
+      <c r="I47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="J47" s="3">
+        <v>41.054657326085888</v>
+      </c>
+      <c r="K47" s="3">
+        <v>112.74524087217139</v>
+      </c>
+      <c r="L47" s="3">
+        <v>0.96544035674470452</v>
+      </c>
+      <c r="O47" s="2"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+    </row>
+    <row r="48" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="E48" s="3">
+        <v>45.94051546096776</v>
+      </c>
+      <c r="F48" s="3">
+        <v>120.465443012229</v>
+      </c>
+      <c r="I48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="J48" s="3">
+        <v>40.579964039446232</v>
+      </c>
+      <c r="K48" s="3">
+        <v>113.53569723847249</v>
+      </c>
+      <c r="L48" s="3">
+        <v>0.96644295302013428</v>
+      </c>
+      <c r="O48" s="2"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+    </row>
+    <row r="49" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="E49" s="3">
+        <v>45.873737860402542</v>
+      </c>
+      <c r="F49" s="3">
+        <v>118.18891373484389</v>
+      </c>
+      <c r="I49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="J49" s="3">
+        <v>40.327379084864383</v>
+      </c>
+      <c r="K49" s="3">
+        <v>116.32759317547161</v>
+      </c>
+      <c r="L49" s="3">
+        <v>0.97345132743362839</v>
+      </c>
+      <c r="O49" s="2"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+    </row>
+    <row r="50" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="E50" s="3">
+        <v>45.718521960759482</v>
+      </c>
+      <c r="F50" s="3">
+        <v>123.307718937779</v>
+      </c>
+      <c r="I50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="J50" s="3">
+        <v>40.999269404312088</v>
+      </c>
+      <c r="K50" s="3">
+        <v>113.5839904685852</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0.96452328159645229</v>
+      </c>
+      <c r="O50" s="2"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+    </row>
+    <row r="51" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="E51" s="3">
+        <v>46.281516569784777</v>
+      </c>
+      <c r="F51" s="3">
+        <v>117.95931199561259</v>
+      </c>
+      <c r="I51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="J51" s="3">
+        <v>41.311010862189057</v>
+      </c>
+      <c r="K51" s="3">
+        <v>111.17919496771</v>
+      </c>
+      <c r="L51" s="3">
+        <v>0.95847362514029166</v>
+      </c>
+      <c r="O51" s="2"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+    </row>
+    <row r="52" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="E52" s="3">
+        <v>46.069720668952193</v>
+      </c>
+      <c r="F52" s="3">
+        <v>116.7572158954174</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="J52" s="3">
+        <v>40.970167039782339</v>
+      </c>
+      <c r="K52" s="3">
+        <v>111.70684844691991</v>
+      </c>
+      <c r="L52" s="3">
+        <v>0.96881959910913151</v>
+      </c>
+      <c r="O52" s="2"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+    </row>
+    <row r="53" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E53" s="3">
+        <v>45.875300855523633</v>
+      </c>
+      <c r="F53" s="3">
+        <v>119.0700686031209</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="J53" s="3">
+        <v>40.67501829605483</v>
+      </c>
+      <c r="K53" s="3">
+        <v>111.6767627333286</v>
+      </c>
+      <c r="L53" s="3">
+        <v>0.96881959910913151</v>
+      </c>
+      <c r="O53" s="2"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+    </row>
+    <row r="54" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="E54" s="3">
+        <v>46.081990204894879</v>
+      </c>
+      <c r="F54" s="3">
+        <v>120.2809559079771</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J54" s="3">
+        <v>41.217747261290057</v>
+      </c>
+      <c r="K54" s="3">
+        <v>111.4633441186561</v>
+      </c>
+      <c r="L54" s="3">
+        <v>0.96802646085997779</v>
+      </c>
+      <c r="O54" s="2"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+    </row>
+    <row r="56" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>46.030772659873563</v>
+      </c>
+      <c r="F56" s="3">
+        <f>AVERAGE(F5:F54)</f>
+        <v>120.14062877929621</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="3">
+        <f>AVERAGE(J5:J54)</f>
+        <v>40.894951755809799</v>
+      </c>
+      <c r="K56" s="3">
+        <f>AVERAGE(K5:K54)</f>
+        <v>111.83629284185935</v>
+      </c>
+      <c r="L56" s="3">
+        <f>AVERAGE(L5:L54)</f>
+        <v>0.96987822088116016</v>
+      </c>
+      <c r="O56" s="2"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+    </row>
+    <row r="57" spans="4:18" x14ac:dyDescent="0.25">
+      <c r="D57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>0.25093706676229333</v>
+      </c>
+      <c r="F57" s="3">
+        <f>_xlfn.STDEV.S(F5:F54)</f>
+        <v>2.2688285249408473</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J57" s="3">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>0.30524315706513966</v>
+      </c>
+      <c r="K57" s="3">
+        <f>_xlfn.STDEV.S(K5:K54)</f>
+        <v>2.2670516403867644</v>
+      </c>
+      <c r="L57" s="3">
+        <f>_xlfn.STDEV.S(L5:L54)</f>
+        <v>5.9892995808688019E-3</v>
+      </c>
+      <c r="O57" s="2"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new value-driven dataset (only big cities)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-14.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-14.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="neg vs pos" sheetId="1" r:id="rId1"/>
     <sheet name="hybrid model" sheetId="2" r:id="rId2"/>
+    <sheet name="big vs small" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -3534,8 +3535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:W57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5144,4 +5145,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test-14: big vs small (44 value-drivent)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-14.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-14.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>Значимость</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-44.csv)</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Small</t>
   </si>
 </sst>
 </file>
@@ -821,6 +830,400 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'big vs small'!$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Big</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'big vs small'!$I$5:$I$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>library</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cultureorg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>musartschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'big vs small'!$J$5:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.23269644597828279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21335492274555701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19015409079792481</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1411649960065024</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.11003988386569021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11258966060604279</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DC5-40E7-9FD3-A9CEAFA9C353}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'big vs small'!$K$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Small</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'big vs small'!$I$5:$I$10</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>library</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cultureorg</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>musartschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'big vs small'!$K$5:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2538639894384162</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25514320812710739</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2111669350124076</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1034524573973921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1203987109236489</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.5974699101027682E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0DC5-40E7-9FD3-A9CEAFA9C353}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="2009885104"/>
+        <c:axId val="2017378784"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2009885104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2017378784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2017378784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2009885104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -901,6 +1304,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
@@ -1421,6 +1864,525 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1988,6 +2950,41 @@
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2275,7 +3272,7 @@
   <dimension ref="C3:S57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:R9"/>
+      <selection activeCell="Q3" sqref="Q3:S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,8 +4532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:W57"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5149,12 +6146,725 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C3:K57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>360.84685410052907</v>
+      </c>
+      <c r="E5" s="3">
+        <v>940.43321596119904</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.23269644597828279</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.2538639894384162</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>352.56476942239868</v>
+      </c>
+      <c r="E6" s="3">
+        <v>947.67780687830668</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.21335492274555701</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.25514320812710739</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>359.15854012345682</v>
+      </c>
+      <c r="E7" s="3">
+        <v>909.95002839506174</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0.19015409079792481</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.2111669350124076</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="3">
+        <v>376.81408256172841</v>
+      </c>
+      <c r="E8" s="3">
+        <v>806.16466666666656</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.1411649960065024</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.1034524573973921</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>363.48330046296297</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1010.391156790123</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.11003988386569021</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.1203987109236489</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="3">
+        <v>366.84209563492072</v>
+      </c>
+      <c r="E10" s="3">
+        <v>867.68799999999999</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.11258966060604279</v>
+      </c>
+      <c r="K10" s="3">
+        <v>5.5974699101027682E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="3">
+        <v>361.05771596119928</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1048.684996296296</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="3">
+        <v>357.19064135802472</v>
+      </c>
+      <c r="E12" s="3">
+        <v>946.01606419753091</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3">
+        <v>359.6161517416225</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1035.5737664902999</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="3">
+        <v>365.24427314814818</v>
+      </c>
+      <c r="E14" s="3">
+        <v>977.7177567901233</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="3">
+        <v>353.66234490740737</v>
+      </c>
+      <c r="E15" s="3">
+        <v>998.51525987654327</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="3">
+        <v>353.84430771604929</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1132.9802276895939</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="3">
+        <v>345.03419991181659</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1133.247253880071</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>360.36661481481491</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1034.592018253968</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="3">
+        <v>367.67591340387997</v>
+      </c>
+      <c r="E19" s="3">
+        <v>872.91008835978835</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="3">
+        <v>360.36771060405653</v>
+      </c>
+      <c r="E20" s="3">
+        <v>1024.303163580247</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="3">
+        <v>362.71350390211637</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1024.6941012345681</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3">
+        <v>362.34572986111112</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1011.9885820987651</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="3">
+        <v>354.91285385802468</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1004.941218518518</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="3">
+        <v>368.86976192680771</v>
+      </c>
+      <c r="E24" s="3">
+        <v>894.56752098765435</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="3">
+        <v>368.38611682098758</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1051.594319753086</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="3">
+        <v>374.35025185185191</v>
+      </c>
+      <c r="E26" s="3">
+        <v>920.81698487654307</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="3">
+        <v>364.98429212962969</v>
+      </c>
+      <c r="E27" s="3">
+        <v>959.24943518518501</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="3">
+        <v>366.13523236331571</v>
+      </c>
+      <c r="E28" s="3">
+        <v>909.03358148148141</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>355.35431395502638</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1055.760293209876</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="3">
+        <v>355.7241125881834</v>
+      </c>
+      <c r="E30" s="3">
+        <v>961.64443721340376</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="3">
+        <v>347.98193710317457</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1057.309517283951</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="3">
+        <v>369.47387515432092</v>
+      </c>
+      <c r="E32" s="3">
+        <v>946.83247345679001</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="3">
+        <v>363.89312592592591</v>
+      </c>
+      <c r="E33" s="3">
+        <v>886.73024382716039</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="3">
+        <v>365.41125416666671</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1014.116654320988</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="3">
+        <v>352.093384303351</v>
+      </c>
+      <c r="E35" s="3">
+        <v>995.00101666666671</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="3">
+        <v>371.90759634038801</v>
+      </c>
+      <c r="E36" s="3">
+        <v>970.46206234567865</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="3">
+        <v>359.74659581128742</v>
+      </c>
+      <c r="E37" s="3">
+        <v>957.42938721340363</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="3">
+        <v>363.52721836419761</v>
+      </c>
+      <c r="E38" s="3">
+        <v>955.65135679012349</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="3">
+        <v>365.56453873456792</v>
+      </c>
+      <c r="E39" s="3">
+        <v>902.84629197530842</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="3">
+        <v>368.00219274691358</v>
+      </c>
+      <c r="E40" s="3">
+        <v>923.14480123456769</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="3">
+        <v>369.11305941358029</v>
+      </c>
+      <c r="E41" s="3">
+        <v>885.06237654320978</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="3">
+        <v>366.46058996913581</v>
+      </c>
+      <c r="E42" s="3">
+        <v>881.01053333333323</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="3">
+        <v>366.19830213844801</v>
+      </c>
+      <c r="E43" s="3">
+        <v>906.05684259259249</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>342.94789691358022</v>
+      </c>
+      <c r="E44" s="3">
+        <v>999.75947407407398</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="3">
+        <v>355.40306018518521</v>
+      </c>
+      <c r="E45" s="3">
+        <v>987.14542222222224</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="3">
+        <v>364.68318487654318</v>
+      </c>
+      <c r="E46" s="3">
+        <v>871.1168148148148</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="3">
+        <v>366.21778472222218</v>
+      </c>
+      <c r="E47" s="3">
+        <v>869.61953888888877</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="3">
+        <v>371.73704481922402</v>
+      </c>
+      <c r="E48" s="3">
+        <v>936.47914417989398</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="3">
+        <v>372.53701783509712</v>
+      </c>
+      <c r="E49" s="3">
+        <v>917.07070767195762</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="3">
+        <v>352.12613780864189</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1060.9229123456789</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="3">
+        <v>370.8018324074074</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1016.914575308642</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="3">
+        <v>366.52374389329822</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1007.207425044092</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="3">
+        <v>361.1063851851851</v>
+      </c>
+      <c r="E53" s="3">
+        <v>967.27913148148139</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="3">
+        <v>359.08989900793648</v>
+      </c>
+      <c r="E54" s="3">
+        <v>881.29823950617288</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="3">
+        <f>AVERAGE(D5:D54)</f>
+        <v>362.20186685912705</v>
+      </c>
+      <c r="E56" s="3">
+        <f>AVERAGE(E5:E54)</f>
+        <v>965.55205775573165</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="3">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>7.4151405044410952</v>
+      </c>
+      <c r="E57" s="3">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>70.749819976251331</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>